<commit_message>
packages added in blogspot
</commit_message>
<xml_diff>
--- a/TourPackageList.xlsx
+++ b/TourPackageList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="23">
   <si>
     <t>Tour Packages</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,6 +536,9 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -553,6 +556,9 @@
       <c r="E5" t="s">
         <v>14</v>
       </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -570,6 +576,9 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -587,6 +596,9 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -624,6 +636,9 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -641,6 +656,9 @@
       <c r="E10" t="s">
         <v>14</v>
       </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -658,6 +676,9 @@
       <c r="E11" t="s">
         <v>14</v>
       </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -672,6 +693,9 @@
       <c r="E12" t="s">
         <v>14</v>
       </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -689,6 +713,9 @@
       <c r="E13" t="s">
         <v>14</v>
       </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -706,6 +733,9 @@
       <c r="E14" t="s">
         <v>14</v>
       </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -720,6 +750,9 @@
       <c r="E15" t="s">
         <v>14</v>
       </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -738,7 +771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -749,6 +782,9 @@
         <v>14</v>
       </c>
       <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated sql and camiguin
</commit_message>
<xml_diff>
--- a/TourPackageList.xlsx
+++ b/TourPackageList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="24">
   <si>
     <t>Tour Packages</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Samal Island Hopping Package</t>
+  </si>
+  <si>
+    <t>adsriver</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +463,7 @@
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,8 +482,11 @@
       <c r="F1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,8 +505,11 @@
       <c r="F2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -520,7 +529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -539,8 +548,11 @@
       <c r="F4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -559,8 +571,11 @@
       <c r="F5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -579,8 +594,11 @@
       <c r="F6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -600,7 +618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -619,8 +637,11 @@
       <c r="F8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -639,8 +660,11 @@
       <c r="F9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -659,8 +683,11 @@
       <c r="F10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -679,8 +706,11 @@
       <c r="F11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -696,8 +726,11 @@
       <c r="F12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -716,8 +749,11 @@
       <c r="F13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -736,8 +772,11 @@
       <c r="F14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -753,8 +792,11 @@
       <c r="F15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -770,8 +812,11 @@
       <c r="F16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -785,6 +830,9 @@
         <v>14</v>
       </c>
       <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>